<commit_message>
new xlsx tasks template
</commit_message>
<xml_diff>
--- a/xls/PM_items.xlsx
+++ b/xls/PM_items.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dp/pm/xls/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A67E23-0724-0E4A-B5F1-93A02C730F5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4EF5CC-D3F9-0F4D-896E-E176A0CADC48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12540" yWindow="2800" windowWidth="28800" windowHeight="15700" activeTab="1" xr2:uid="{9DBAF000-1E47-A24E-B53F-157DA7A2A96D}"/>
+    <workbookView xWindow="12540" yWindow="2800" windowWidth="34120" windowHeight="19640" activeTab="1" xr2:uid="{9DBAF000-1E47-A24E-B53F-157DA7A2A96D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_20210310_085338" localSheetId="0">Hoja1!$A$1:$B$395</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$395</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$1:$G$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hoja2!$A$1:$G$132</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4701,10 +4701,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00C047F-BE6B-4948-8F0F-346F2C3C5904}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6481,7 +6482,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>302</v>
       </c>
@@ -6501,7 +6502,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>302</v>
       </c>
@@ -6521,7 +6522,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>302</v>
       </c>
@@ -6541,7 +6542,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>302</v>
       </c>
@@ -6561,7 +6562,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>302</v>
       </c>
@@ -6581,7 +6582,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>302</v>
       </c>
@@ -6601,7 +6602,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>302</v>
       </c>
@@ -6621,7 +6622,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>302</v>
       </c>
@@ -6641,7 +6642,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>302</v>
       </c>
@@ -6661,7 +6662,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>302</v>
       </c>
@@ -6681,7 +6682,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>302</v>
       </c>
@@ -6701,7 +6702,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>301</v>
       </c>
@@ -6721,7 +6722,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>301</v>
       </c>
@@ -6741,7 +6742,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>301</v>
       </c>
@@ -6761,7 +6762,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>301</v>
       </c>
@@ -6781,7 +6782,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>301</v>
       </c>
@@ -6801,7 +6802,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>301</v>
       </c>
@@ -6821,7 +6822,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>301</v>
       </c>
@@ -6841,7 +6842,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>301</v>
       </c>
@@ -6861,7 +6862,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>301</v>
       </c>
@@ -6881,7 +6882,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>301</v>
       </c>
@@ -6901,7 +6902,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>301</v>
       </c>
@@ -6921,7 +6922,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>301</v>
       </c>
@@ -6941,7 +6942,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>301</v>
       </c>
@@ -6961,7 +6962,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>301</v>
       </c>
@@ -6981,7 +6982,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>301</v>
       </c>
@@ -7001,7 +7002,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>301</v>
       </c>
@@ -7021,7 +7022,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>301</v>
       </c>
@@ -7041,7 +7042,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>301</v>
       </c>
@@ -7061,7 +7062,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>301</v>
       </c>
@@ -7081,7 +7082,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>301</v>
       </c>
@@ -7101,7 +7102,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>301</v>
       </c>
@@ -7121,7 +7122,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>301</v>
       </c>
@@ -7141,7 +7142,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>301</v>
       </c>
@@ -7161,7 +7162,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>301</v>
       </c>
@@ -7181,7 +7182,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>301</v>
       </c>
@@ -7201,7 +7202,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>301</v>
       </c>
@@ -7221,7 +7222,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>301</v>
       </c>
@@ -7241,7 +7242,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>301</v>
       </c>
@@ -7261,7 +7262,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>301</v>
       </c>
@@ -7281,7 +7282,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>301</v>
       </c>
@@ -7301,7 +7302,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>301</v>
       </c>
@@ -7321,7 +7322,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>301</v>
       </c>
@@ -7341,7 +7342,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>301</v>
       </c>
@@ -7362,7 +7363,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G98" xr:uid="{251DF630-603F-434C-81FC-2CF3B1A025CD}"/>
+  <autoFilter ref="A1:G132" xr:uid="{251DF630-603F-434C-81FC-2CF3B1A025CD}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="TECHNIP ITALY"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>